<commit_message>
Update New Microsoft Excel Worksheet.xlsx
ADDED SERVICES IN EXCEL SHEET
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\BOOT CAMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\GladDemo\GladDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FCD309-F774-40D6-87C4-ECA3FB11C5E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70750B40-42D6-4CC5-8652-5F2010CF00CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -93,31 +93,34 @@
     <t xml:space="preserve">Create the home page component with Login, Register, Flight search options using CSS/Bootstrap/angular material </t>
   </si>
   <si>
-    <t>Create Register page for a new user and take required inputs (validate) . (Same style as home page)</t>
-  </si>
-  <si>
-    <t>Create Login page for a registered user , take required inputs and validate login credentials from DB  . (Same style as home page)</t>
-  </si>
-  <si>
     <t>Create Login page for Admin , take required inputs ( Email, password) and validate credentials .</t>
   </si>
   <si>
-    <t>Create a flight search page for user to input, source, destination, date, number of passengers ,type of trip from user and show available flights. (route to home page)</t>
-  </si>
-  <si>
     <t>Create a seat matrix to show to user the available and booked seats when the user selects a flight.</t>
   </si>
   <si>
-    <t>Create a payment page and method for a user who has selected seat(s) for a flight and wants to book the seats.</t>
-  </si>
-  <si>
-    <t>Create a method to print booked tickets</t>
-  </si>
-  <si>
     <t>Forgot Password (User)</t>
   </si>
   <si>
     <t>Create a ticket cancellation page for User and check for booking details to cancel a booked ticket</t>
+  </si>
+  <si>
+    <t>Create Login page for a registered user , take required inputs and validate login credentials from DB  . (Same style as home page)  [LOGIN SERVICE]</t>
+  </si>
+  <si>
+    <t>Create a flight search page for user to input, source, destination, date, number of passengers ,type of trip from user and show available flights. (route to home page) [SEARCH SERVICE]</t>
+  </si>
+  <si>
+    <t>Create Register page for a new user and take required inputs (validate) . (Same style as home page) [CRUD SERVICE]</t>
+  </si>
+  <si>
+    <t>Create a payment page and method for a user who has selected seat(s) for a flight and wants to book the seats. [PAYMENT SERVICE]</t>
+  </si>
+  <si>
+    <t>Create a method to print booked tickets [PRINT SERVICE]</t>
+  </si>
+  <si>
+    <t>FORGOT PASSWORD SERVICE</t>
   </si>
 </sst>
 </file>
@@ -451,20 +454,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="63.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="24.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -480,7 +483,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -488,7 +491,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -496,7 +499,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -504,7 +507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -512,83 +515,86 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/Aman270399/GladDemo"
This reverts commit 639303ee506bace9f38947812e76551448eb928c, reversing
changes made to 65373cd1fd28b6eb91534b113ba74a565aee428c.
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\Gladiator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D091E7-FEBD-4D40-9FE4-326532C383CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3B79D-90C1-4234-8EC7-7872EF9A40C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,23 +732,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -764,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,59 +772,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/Aman270399/GladDemo""
This reverts commit 6676d1914a2a443365297c495df74607a16ca065.
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\Gladiator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3B79D-90C1-4234-8EC7-7872EF9A40C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D091E7-FEBD-4D40-9FE4-326532C383CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="72" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,23 +732,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -764,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,59 +772,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Merge branch 'master' of https://github.com/Aman270399/GladDemo"""
This reverts commit b8f8dc2c8022a107e4717534e582cf6a1691eeb8.
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\Gladiator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D091E7-FEBD-4D40-9FE4-326532C383CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3B79D-90C1-4234-8EC7-7872EF9A40C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,23 +732,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -764,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,59 +772,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Merge branch 'master' of https://github.com/Aman270399/GladDemo""""
This reverts commit 9c10bed03d109eee2c9d23025f46b2e552e397b1.
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aman\Desktop\Gladiator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3B79D-90C1-4234-8EC7-7872EF9A40C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D091E7-FEBD-4D40-9FE4-326532C383CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="72" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,23 +732,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -764,7 +764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -772,59 +772,59 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>